<commit_message>
minor fix for date
</commit_message>
<xml_diff>
--- a/scheduler/data/Polishing Production Orders JUNHO2017_20180409.xlsx
+++ b/scheduler/data/Polishing Production Orders JUNHO2017_20180409.xlsx
@@ -620,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -712,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="8">
-        <v>42881.333333333336</v>
+        <v>43246.333333333336</v>
       </c>
       <c r="K2" s="8">
-        <v>42887.382638888892</v>
+        <v>43252.382638888892</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="8">
-        <v>42886.335416666669</v>
+        <v>43251.335416666669</v>
       </c>
       <c r="K3" s="8">
-        <v>42887.383333333331</v>
+        <v>43252.383333333331</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -780,10 +780,10 @@
         <v>0.1277777777777778</v>
       </c>
       <c r="J4" s="8">
-        <v>42887.383333333331</v>
+        <v>43252.383333333331</v>
       </c>
       <c r="K4" s="8">
-        <v>42887.573611111111</v>
+        <v>43252.573611111111</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -812,10 +812,10 @@
         <v>0.35833333333333334</v>
       </c>
       <c r="J5" s="8">
-        <v>42891.350694444445</v>
+        <v>43256.350694444445</v>
       </c>
       <c r="K5" s="8">
-        <v>42892.256944444445</v>
+        <v>43257.256944444445</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,10 +845,10 @@
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="8">
-        <v>42892.364583333336</v>
+        <v>43257.364583333336</v>
       </c>
       <c r="K6" s="8">
-        <v>42892.619444444441</v>
+        <v>43257.619444444441</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -880,10 +880,10 @@
         <v>8.1944444444444445E-2</v>
       </c>
       <c r="J7" s="8">
-        <v>42893.25</v>
+        <v>43258.25</v>
       </c>
       <c r="K7" s="8">
-        <v>42893.333333333336</v>
+        <v>43258.333333333336</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -912,10 +912,10 @@
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="J8" s="8">
-        <v>42893.340277777781</v>
+        <v>43258.340277777781</v>
       </c>
       <c r="K8" s="8">
-        <v>42893.387499999997</v>
+        <v>43258.387499999997</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -944,10 +944,10 @@
         <v>2.1527777777777781E-2</v>
       </c>
       <c r="J9" s="8">
-        <v>42893.387499999997</v>
+        <v>43258.387499999997</v>
       </c>
       <c r="K9" s="8">
-        <v>42893.40902777778</v>
+        <v>43258.40902777778</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -976,10 +976,10 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="J10" s="8">
-        <v>42893.429166666669</v>
+        <v>43258.429166666669</v>
       </c>
       <c r="K10" s="8">
-        <v>42893.436111111114</v>
+        <v>43258.436111111114</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1008,10 +1008,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="J11" s="8">
-        <v>42893.436111111114</v>
+        <v>43258.436111111114</v>
       </c>
       <c r="K11" s="8">
-        <v>42893.457638888889</v>
+        <v>43258.457638888889</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1044,10 +1044,10 @@
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="J12" s="8">
-        <v>42893.5</v>
+        <v>43258.5</v>
       </c>
       <c r="K12" s="8">
-        <v>42893.541666666664</v>
+        <v>43258.541666666664</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,10 +1079,10 @@
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="J13" s="8">
-        <v>42893.5</v>
+        <v>43258.5</v>
       </c>
       <c r="K13" s="8">
-        <v>42893.541666666664</v>
+        <v>43258.541666666664</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1114,10 +1114,10 @@
         <v>1.4583333333333332E-2</v>
       </c>
       <c r="J14" s="8">
-        <v>42893.541666666664</v>
+        <v>43258.541666666664</v>
       </c>
       <c r="K14" s="8">
-        <v>42893.587500000001</v>
+        <v>43258.587500000001</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,10 +1146,10 @@
         <v>2.6388888888888889E-2</v>
       </c>
       <c r="J15" s="8">
-        <v>42893.583333333336</v>
+        <v>43258.583333333336</v>
       </c>
       <c r="K15" s="8">
-        <v>42893.613888888889</v>
+        <v>43258.613888888889</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1178,10 +1178,10 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="J16" s="8">
-        <v>42893.613888888889</v>
+        <v>43258.613888888889</v>
       </c>
       <c r="K16" s="8">
-        <v>42894.585416666669</v>
+        <v>43259.585416666669</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,10 +1213,10 @@
         <v>4.5833333333333337E-2</v>
       </c>
       <c r="J17" s="8">
-        <v>42895.286805555559</v>
+        <v>43260.286805555559</v>
       </c>
       <c r="K17" s="8">
-        <v>42895.314583333333</v>
+        <v>43260.314583333333</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1245,10 +1245,10 @@
         <v>0.54652777777777783</v>
       </c>
       <c r="J18" s="8">
-        <v>42895.34097222222</v>
+        <v>43260.34097222222</v>
       </c>
       <c r="K18" s="8">
-        <v>42898.572916666664</v>
+        <v>43263.572916666664</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1277,10 +1277,10 @@
         <v>0.12013888888888889</v>
       </c>
       <c r="J19" s="8">
-        <v>42898.573611111111</v>
+        <v>43263.573611111111</v>
       </c>
       <c r="K19" s="8">
-        <v>42898.693749999999</v>
+        <v>43263.693749999999</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1309,10 +1309,10 @@
         <v>7.7083333333333337E-2</v>
       </c>
       <c r="J20" s="8">
-        <v>42898.693055555559</v>
+        <v>43263.693055555559</v>
       </c>
       <c r="K20" s="8">
-        <v>42898.779166666667</v>
+        <v>43263.779166666667</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1341,10 +1341,10 @@
         <v>0.1673611111111111</v>
       </c>
       <c r="J21" s="8">
-        <v>42899.491666666669</v>
+        <v>43264.491666666669</v>
       </c>
       <c r="K21" s="8">
-        <v>42899.720833333333</v>
+        <v>43264.720833333333</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1376,10 +1376,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="J22" s="8">
-        <v>42900.25</v>
+        <v>43265.25</v>
       </c>
       <c r="K22" s="8">
-        <v>42900.333333333336</v>
+        <v>43265.333333333336</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1411,10 +1411,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J23" s="8">
-        <v>42900.5</v>
+        <v>43265.5</v>
       </c>
       <c r="K23" s="8">
-        <v>42900.541666666664</v>
+        <v>43265.541666666664</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1443,10 +1443,10 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="J24" s="8">
-        <v>42900.715277777781</v>
+        <v>43265.715277777781</v>
       </c>
       <c r="K24" s="8">
-        <v>42900.779166666667</v>
+        <v>43265.779166666667</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1475,10 +1475,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J25" s="8">
-        <v>42902.5</v>
+        <v>43267.5</v>
       </c>
       <c r="K25" s="8">
-        <v>42902.541666666664</v>
+        <v>43267.541666666664</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1507,10 +1507,10 @@
         <v>0.12916666666666668</v>
       </c>
       <c r="J26" s="8">
-        <v>42902.64166666667</v>
+        <v>43267.64166666667</v>
       </c>
       <c r="K26" s="8">
-        <v>42902.770833333336</v>
+        <v>43267.770833333336</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1542,10 +1542,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="J27" s="8">
-        <v>42905.25</v>
+        <v>43270.25</v>
       </c>
       <c r="K27" s="8">
-        <v>42905.333333333336</v>
+        <v>43270.333333333336</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1574,10 +1574,10 @@
         <v>0.30555555555555552</v>
       </c>
       <c r="J28" s="8">
-        <v>42905.333333333336</v>
+        <v>43270.333333333336</v>
       </c>
       <c r="K28" s="8">
-        <v>42905.6875</v>
+        <v>43270.6875</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>